<commit_message>
Final update Sprint 3
</commit_message>
<xml_diff>
--- a/Phase 2/Sprint3/BurnDown_Chart.xlsx
+++ b/Phase 2/Sprint3/BurnDown_Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Desktop\SE2223_59797_60441_60677_60816_60971\Phase 2\Sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB003D1-48CF-4A62-87C7-EB8D4767C9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C637A205-21FE-40F0-834B-98EE81CFC81F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -829,7 +829,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -838,7 +838,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -942,16 +942,16 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2206,7 +2206,7 @@
   <dimension ref="B1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2333,7 +2333,9 @@
       <c r="E6" s="3">
         <v>1</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="5"/>
@@ -2364,7 +2366,9 @@
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="8"/>
+      <c r="I7" s="8">
+        <v>1</v>
+      </c>
       <c r="J7" s="23"/>
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
@@ -2561,7 +2565,7 @@
       </c>
       <c r="F16" s="12">
         <f t="shared" ref="F16:I16" si="0">SUM(F6:F15)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16" s="12">
         <f t="shared" si="0"/>
@@ -2573,7 +2577,7 @@
       </c>
       <c r="I16" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J16" s="23"/>
       <c r="K16" s="23"/>
@@ -2601,19 +2605,19 @@
       </c>
       <c r="F17" s="13">
         <f t="shared" ref="F17:H17" si="1">E17-SUM(F6:F15)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G17" s="13">
         <f>F17-SUM(G6:G15)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H17" s="13">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="36">
         <f>H17-SUM(I6:I15)</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="J17" s="23"/>
       <c r="K17" s="23"/>

</xml_diff>